<commit_message>
[DROOLS-3888] group dtables in KieBases by packages instead of folders (#2318)
</commit_message>
<xml_diff>
--- a/drools-decisiontables/src/test/resources/org/drools/decisiontable/integrationtests/xlsx/incrementalBuild.dtable.xlsx
+++ b/drools-decisiontables/src/test/resources/org/drools/decisiontable/integrationtests/xlsx/incrementalBuild.dtable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="601" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tables" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,76 +17,81 @@
     <definedName function="false" hidden="false" name="Excel_BuiltIn__FilterDatabase_2" vbProcedure="false">Lists!$A$5:$A$7</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
-    <t>RuleSet</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>RuleTable Test</t>
-  </si>
-  <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t>CONDITION</t>
-  </si>
-  <si>
-    <t>ACTION</t>
-  </si>
-  <si>
-    <t>$s : String</t>
-  </si>
-  <si>
-    <t>this ==</t>
-  </si>
-  <si>
-    <t>System.out.println( $s );</t>
-  </si>
-  <si>
-    <t>Rule Names</t>
-  </si>
-  <si>
-    <t>Rule1</t>
-  </si>
-  <si>
-    <t>Hello</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Insurance Types</t>
-  </si>
-  <si>
-    <t>Pricing Brackets</t>
-  </si>
-  <si>
-    <t>Location risk</t>
-  </si>
-  <si>
-    <t>COMPREHENSIVE</t>
-  </si>
-  <si>
-    <t>LOW</t>
-  </si>
-  <si>
-    <t>FIRE_THEFT</t>
-  </si>
-  <si>
-    <t>MED</t>
-  </si>
-  <si>
-    <t>THIRD_PARTY</t>
-  </si>
-  <si>
-    <t>HIGH</t>
+    <t xml:space="preserve">RuleSet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">org.drools.decisiontable.integrationtests.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RuleTable Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONDITION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$s : String</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this ==</t>
+  </si>
+  <si>
+    <t xml:space="preserve">System.out.println( $s );</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rule Names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rule1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hello</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insurance Types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pricing Brackets</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location risk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMPREHENSIVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIRE_THEFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THIRD_PARTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIGH</t>
   </si>
 </sst>
 </file>
@@ -94,7 +99,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="8">
@@ -401,13 +406,13 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -419,23 +424,23 @@
   </sheetPr>
   <dimension ref="A1:IS10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.1"/>
+  <sheetFormatPr defaultRowHeight="14.1" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="0.142857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="23.8316326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.1275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="20.1224489795918"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.6938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.4081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.6938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="17.4030612244898"/>
-    <col collapsed="false" hidden="false" max="253" min="10" style="1" width="9.13265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="254" style="0" width="9.13265306122449"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="0.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="20.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="253" min="10" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="254" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1771,7 +1776,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.15" right="0.140277777777778" top="0.179861111111111" bottom="0.2" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1786,18 +1791,18 @@
   </sheetPr>
   <dimension ref="A4:E7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.9795918367347"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.2704081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.72959183673469"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.73"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1847,7 +1852,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>